<commit_message>
Work on singleM cluster picking
</commit_message>
<xml_diff>
--- a/Data/N_cycle/Nitrogen_ko_gene_list.xlsx
+++ b/Data/N_cycle/Nitrogen_ko_gene_list.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maria Vega\Dropbox\PC\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uqoshopi\Dropbox\Olga Shopina\Shotgun\GSVeasy090823\Data\N_cycle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F182E00-415B-413D-995E-EDA230D9AB2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{647F9A15-C92D-404B-9287-057A09093560}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{5B114E74-39B1-4A06-BD9B-D4D0D6C33FF4}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5B114E74-39B1-4A06-BD9B-D4D0D6C33FF4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="277">
   <si>
     <t>KO</t>
   </si>
@@ -870,12 +871,144 @@
   <si>
     <t>Anmx&lt;-c("hzo","hzsA","hzsB","hzsC")</t>
   </si>
+  <si>
+    <t>anfD</t>
+  </si>
+  <si>
+    <t>anfH</t>
+  </si>
+  <si>
+    <t>anfK</t>
+  </si>
+  <si>
+    <t>asnB</t>
+  </si>
+  <si>
+    <t>gdhA</t>
+  </si>
+  <si>
+    <t>glnA</t>
+  </si>
+  <si>
+    <t>glsA</t>
+  </si>
+  <si>
+    <t>gltB</t>
+  </si>
+  <si>
+    <t>gltD</t>
+  </si>
+  <si>
+    <t>gltS</t>
+  </si>
+  <si>
+    <t>gudB</t>
+  </si>
+  <si>
+    <t>hcp</t>
+  </si>
+  <si>
+    <t>narC</t>
+  </si>
+  <si>
+    <t>narJ</t>
+  </si>
+  <si>
+    <t>nod</t>
+  </si>
+  <si>
+    <t>nrfB</t>
+  </si>
+  <si>
+    <t>nrfC</t>
+  </si>
+  <si>
+    <t>nrfD</t>
+  </si>
+  <si>
+    <t>ureA</t>
+  </si>
+  <si>
+    <t>ureB</t>
+  </si>
+  <si>
+    <t>ureC</t>
+  </si>
+  <si>
+    <t>Pathway</t>
+  </si>
+  <si>
+    <t>Gene</t>
+  </si>
+  <si>
+    <t>Nitrification/Commamox</t>
+  </si>
+  <si>
+    <t>Ammonia assimilation</t>
+  </si>
+  <si>
+    <t>Anammox /Commamox</t>
+  </si>
+  <si>
+    <t>Anammox</t>
+  </si>
+  <si>
+    <t>Anaerobic ammonium oxidation</t>
+  </si>
+  <si>
+    <t>Nitrate reduction</t>
+  </si>
+  <si>
+    <t>Denitrification</t>
+  </si>
+  <si>
+    <t>Nitrate reduction (narG) / Nitrification (nxrA) /Commamox</t>
+  </si>
+  <si>
+    <t>Nitrate reduction (narH) / Nitrification (nxrB) /Commamox</t>
+  </si>
+  <si>
+    <t>Denitrification/DNRA</t>
+  </si>
+  <si>
+    <t>Nitrate/Nitrite reduction</t>
+  </si>
+  <si>
+    <t>DNRA</t>
+  </si>
+  <si>
+    <t>Dissimilatory nitrate reduction</t>
+  </si>
+  <si>
+    <t>Assimilatory nitrate reduction</t>
+  </si>
+  <si>
+    <t>Nitrite reduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Glutamate metabolism</t>
+  </si>
+  <si>
+    <t>Denitrification/nitrate reduction</t>
+  </si>
+  <si>
+    <t>Reaction</t>
+  </si>
+  <si>
+    <t>Enzyme</t>
+  </si>
+  <si>
+    <t>Gene group</t>
+  </si>
+  <si>
+    <t>General function</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -940,6 +1073,48 @@
       <i/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1103,7 +1278,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1195,6 +1370,39 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2887,8 +3095,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{129D74BC-0292-48BA-99B6-832221E100BA}">
   <dimension ref="R2:AF18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R7" workbookViewId="0">
-      <selection activeCell="T8" sqref="T8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21.5" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -3154,8 +3362,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{247BCA96-EF79-4C07-878C-3C9DB32BD331}">
   <dimension ref="A1:F91"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView topLeftCell="A65" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B73" sqref="B73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3209,7 +3417,7 @@
       <c r="B4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="35" t="s">
         <v>100</v>
       </c>
       <c r="D4" s="28"/>
@@ -3225,7 +3433,7 @@
       <c r="B5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="35" t="s">
         <v>101</v>
       </c>
       <c r="D5" s="29"/>
@@ -3240,7 +3448,7 @@
       <c r="B6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="28" t="s">
+      <c r="C6" s="35" t="s">
         <v>102</v>
       </c>
       <c r="D6" s="29"/>
@@ -3252,7 +3460,7 @@
       <c r="B7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="28" t="s">
+      <c r="C7" s="35" t="s">
         <v>103</v>
       </c>
       <c r="D7" s="29"/>
@@ -3268,7 +3476,7 @@
       <c r="B8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="28" t="s">
+      <c r="C8" s="35" t="s">
         <v>104</v>
       </c>
       <c r="D8" s="29"/>
@@ -3283,7 +3491,7 @@
       <c r="B9" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="28" t="s">
+      <c r="C9" s="35" t="s">
         <v>105</v>
       </c>
       <c r="D9" s="29"/>
@@ -3295,7 +3503,7 @@
       <c r="B10" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="28" t="s">
+      <c r="C10" s="35" t="s">
         <v>106</v>
       </c>
       <c r="D10" s="29"/>
@@ -3307,7 +3515,7 @@
       <c r="B11" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="28" t="s">
+      <c r="C11" s="35" t="s">
         <v>107</v>
       </c>
       <c r="D11" s="28"/>
@@ -3324,7 +3532,7 @@
       <c r="B14" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="19"/>
+      <c r="C14" s="36"/>
       <c r="D14" s="19"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
@@ -3334,7 +3542,7 @@
       <c r="B15" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="30"/>
+      <c r="C15" s="37"/>
       <c r="D15" s="30"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
@@ -3344,7 +3552,7 @@
       <c r="B16" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="36" t="s">
         <v>108</v>
       </c>
       <c r="D16" s="31"/>
@@ -3360,7 +3568,7 @@
       <c r="B17" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="36" t="s">
         <v>109</v>
       </c>
       <c r="D17" s="10"/>
@@ -3375,7 +3583,7 @@
       <c r="B18" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C18" s="36" t="s">
         <v>131</v>
       </c>
       <c r="D18" s="10"/>
@@ -3387,7 +3595,7 @@
       <c r="B19" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="36" t="s">
         <v>110</v>
       </c>
       <c r="D19" s="10"/>
@@ -3403,7 +3611,7 @@
       <c r="B20" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="36" t="s">
         <v>111</v>
       </c>
       <c r="D20" s="31"/>
@@ -3418,7 +3626,7 @@
       <c r="B21" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C21" s="36" t="s">
         <v>112</v>
       </c>
       <c r="D21" s="31"/>
@@ -3430,7 +3638,7 @@
       <c r="B22" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="36" t="s">
         <v>132</v>
       </c>
       <c r="D22" s="31"/>
@@ -3442,7 +3650,7 @@
       <c r="B23" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C23" s="36" t="s">
         <v>113</v>
       </c>
       <c r="D23" s="31"/>
@@ -3454,7 +3662,7 @@
       <c r="B24" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="C24" s="36" t="s">
         <v>110</v>
       </c>
       <c r="D24" s="31"/>
@@ -3471,7 +3679,7 @@
       <c r="B27" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="C27" s="19"/>
+      <c r="C27" s="36"/>
       <c r="D27" s="19"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
@@ -3481,17 +3689,17 @@
       <c r="B28" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C28" s="30"/>
+      <c r="C28" s="37"/>
       <c r="D28" s="30"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" ht="27" x14ac:dyDescent="0.35">
       <c r="A29" s="13" t="s">
         <v>43</v>
       </c>
       <c r="B29" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C29" s="36" t="s">
         <v>135</v>
       </c>
       <c r="D29" s="31"/>
@@ -3500,14 +3708,14 @@
         <v>"K00370","K00371","K00374","K02567","K02568","K00362","K00363","K03385","K15876"</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" ht="27" x14ac:dyDescent="0.35">
       <c r="A30" s="13" t="s">
         <v>45</v>
       </c>
       <c r="B30" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="C30" s="10" t="s">
+      <c r="C30" s="36" t="s">
         <v>136</v>
       </c>
       <c r="D30" s="31"/>
@@ -3522,7 +3730,7 @@
       <c r="B31" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="C31" s="10" t="s">
+      <c r="C31" s="36" t="s">
         <v>134</v>
       </c>
       <c r="D31" s="31"/>
@@ -3534,7 +3742,7 @@
       <c r="B32" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="C32" s="10" t="s">
+      <c r="C32" s="36" t="s">
         <v>114</v>
       </c>
       <c r="D32" s="31"/>
@@ -3550,7 +3758,7 @@
       <c r="B33" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C33" s="10" t="s">
+      <c r="C33" s="36" t="s">
         <v>115</v>
       </c>
       <c r="D33" s="10"/>
@@ -3565,7 +3773,7 @@
       <c r="B34" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="C34" s="10" t="s">
+      <c r="C34" s="36" t="s">
         <v>116</v>
       </c>
       <c r="D34" s="31"/>
@@ -3577,7 +3785,7 @@
       <c r="B35" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="C35" s="10" t="s">
+      <c r="C35" s="36" t="s">
         <v>117</v>
       </c>
       <c r="D35" s="31"/>
@@ -3589,7 +3797,7 @@
       <c r="B36" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="C36" s="10" t="s">
+      <c r="C36" s="36" t="s">
         <v>118</v>
       </c>
       <c r="D36" s="31"/>
@@ -3601,19 +3809,19 @@
       <c r="B37" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="C37" s="10" t="s">
+      <c r="C37" s="36" t="s">
         <v>119</v>
       </c>
       <c r="D37" s="10"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="C38" s="10"/>
+      <c r="C38" s="36"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C39" s="10"/>
+      <c r="C39" s="36"/>
     </row>
     <row r="40" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="9" t="s">
@@ -3622,7 +3830,7 @@
       <c r="B40" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="C40" s="10"/>
+      <c r="C40" s="36"/>
       <c r="D40" s="19"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
@@ -3632,17 +3840,17 @@
       <c r="B41" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C41" s="10"/>
+      <c r="C41" s="36"/>
       <c r="D41" s="30"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" ht="27" x14ac:dyDescent="0.35">
       <c r="A42" s="13" t="s">
         <v>43</v>
       </c>
       <c r="B42" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="C42" s="10" t="s">
+      <c r="C42" s="36" t="s">
         <v>138</v>
       </c>
       <c r="D42" s="31"/>
@@ -3651,14 +3859,14 @@
         <v>"K00370","K00371","K00374","K02567","K02568","K00368","K15864","K04561","K02305","K00376"</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" ht="27" x14ac:dyDescent="0.35">
       <c r="A43" s="13" t="s">
         <v>45</v>
       </c>
       <c r="B43" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="C43" s="10" t="s">
+      <c r="C43" s="36" t="s">
         <v>136</v>
       </c>
       <c r="D43" s="31"/>
@@ -3673,7 +3881,7 @@
       <c r="B44" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="C44" s="10" t="s">
+      <c r="C44" s="36" t="s">
         <v>134</v>
       </c>
       <c r="D44" s="31"/>
@@ -3685,7 +3893,7 @@
       <c r="B45" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="C45" s="10" t="s">
+      <c r="C45" s="36" t="s">
         <v>114</v>
       </c>
       <c r="D45" s="31"/>
@@ -3701,7 +3909,7 @@
       <c r="B46" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C46" s="10" t="s">
+      <c r="C46" s="36" t="s">
         <v>115</v>
       </c>
       <c r="D46" s="10"/>
@@ -3716,7 +3924,7 @@
       <c r="B47" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="C47" s="10" t="s">
+      <c r="C47" s="36" t="s">
         <v>120</v>
       </c>
       <c r="D47" s="31"/>
@@ -3728,7 +3936,7 @@
       <c r="B48" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="C48" s="10" t="s">
+      <c r="C48" s="36" t="s">
         <v>121</v>
       </c>
       <c r="D48" s="10"/>
@@ -3740,7 +3948,7 @@
       <c r="B49" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="C49" s="10" t="s">
+      <c r="C49" s="36" t="s">
         <v>122</v>
       </c>
       <c r="D49" s="31"/>
@@ -3752,7 +3960,7 @@
       <c r="B50" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="C50" s="10" t="s">
+      <c r="C50" s="36" t="s">
         <v>123</v>
       </c>
       <c r="D50" s="10"/>
@@ -3764,19 +3972,19 @@
       <c r="B51" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="C51" s="10" t="s">
+      <c r="C51" s="36" t="s">
         <v>124</v>
       </c>
       <c r="D51" s="31"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="C52" s="10"/>
+      <c r="C52" s="36"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C53" s="10"/>
+      <c r="C53" s="36"/>
     </row>
     <row r="54" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A54" s="9" t="s">
@@ -3785,7 +3993,7 @@
       <c r="B54" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="C54" s="10"/>
+      <c r="C54" s="36"/>
       <c r="D54" s="19"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.35">
@@ -3795,7 +4003,7 @@
       <c r="B55" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C55" s="10"/>
+      <c r="C55" s="36"/>
       <c r="D55" s="30"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
@@ -3805,7 +4013,7 @@
       <c r="B56" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="C56" s="10" t="s">
+      <c r="C56" s="36" t="s">
         <v>143</v>
       </c>
       <c r="D56" s="10"/>
@@ -3821,7 +4029,7 @@
       <c r="B57" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="C57" s="10" t="s">
+      <c r="C57" s="36" t="s">
         <v>144</v>
       </c>
       <c r="D57" s="10"/>
@@ -3836,7 +4044,7 @@
       <c r="B58" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="C58" s="10" t="s">
+      <c r="C58" s="36" t="s">
         <v>145</v>
       </c>
       <c r="D58" s="10"/>
@@ -3852,7 +4060,7 @@
       <c r="B59" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="C59" s="10" t="s">
+      <c r="C59" s="36" t="s">
         <v>125</v>
       </c>
       <c r="D59" s="31"/>
@@ -3861,13 +4069,13 @@
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="C60" s="10"/>
+      <c r="C60" s="36"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C61" s="10"/>
+      <c r="C61" s="36"/>
     </row>
     <row r="62" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A62" s="9" t="s">
@@ -3876,7 +4084,7 @@
       <c r="B62" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="C62" s="10"/>
+      <c r="C62" s="36"/>
       <c r="D62" s="10"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.35">
@@ -3886,7 +4094,7 @@
       <c r="B63" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C63" s="10"/>
+      <c r="C63" s="36"/>
       <c r="D63" s="30"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.35">
@@ -3896,7 +4104,7 @@
       <c r="B64" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="C64" s="10" t="s">
+      <c r="C64" s="36" t="s">
         <v>143</v>
       </c>
       <c r="D64" s="10"/>
@@ -3912,7 +4120,7 @@
       <c r="B65" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="C65" s="10" t="s">
+      <c r="C65" s="36" t="s">
         <v>144</v>
       </c>
       <c r="D65" s="10"/>
@@ -3927,7 +4135,7 @@
       <c r="B66" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="C66" s="10" t="s">
+      <c r="C66" s="36" t="s">
         <v>145</v>
       </c>
       <c r="D66" s="10"/>
@@ -3939,7 +4147,7 @@
       <c r="B67" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="C67" s="10" t="s">
+      <c r="C67" s="36" t="s">
         <v>125</v>
       </c>
       <c r="D67" s="31"/>
@@ -3948,14 +4156,14 @@
         <v>"amoA","amoB","amoC","hao","narG_nxrA","narH_nxrB"</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:6" ht="27" x14ac:dyDescent="0.35">
       <c r="A68" s="13" t="s">
         <v>43</v>
       </c>
       <c r="B68" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="C68" s="10" t="s">
+      <c r="C68" s="36" t="s">
         <v>138</v>
       </c>
       <c r="D68" s="31"/>
@@ -3963,29 +4171,29 @@
         <v>148</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:6" ht="27.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A69" s="16" t="s">
         <v>45</v>
       </c>
       <c r="B69" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="C69" s="10" t="s">
+      <c r="C69" s="36" t="s">
         <v>136</v>
       </c>
       <c r="D69" s="31"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C70" s="10"/>
+      <c r="C70" s="36"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C71" s="10"/>
+      <c r="C71" s="36"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A72" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="C72" s="10"/>
+      <c r="C72" s="36"/>
     </row>
     <row r="73" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A73" s="9" t="s">
@@ -3994,7 +4202,7 @@
       <c r="B73" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="C73" s="10"/>
+      <c r="C73" s="36"/>
       <c r="D73" s="10"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.35">
@@ -4004,7 +4212,7 @@
       <c r="B74" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C74" s="10"/>
+      <c r="C74" s="36"/>
       <c r="D74" s="30"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.35">
@@ -4014,7 +4222,7 @@
       <c r="B75" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="C75" s="10" t="s">
+      <c r="C75" s="36" t="s">
         <v>150</v>
       </c>
       <c r="D75" s="31"/>
@@ -4031,7 +4239,7 @@
       <c r="B76" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="C76" s="10" t="s">
+      <c r="C76" s="36" t="s">
         <v>128</v>
       </c>
       <c r="D76" s="32"/>
@@ -4046,7 +4254,7 @@
       <c r="B77" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="C77" s="10" t="s">
+      <c r="C77" s="36" t="s">
         <v>126</v>
       </c>
       <c r="D77" s="32"/>
@@ -4062,7 +4270,7 @@
       <c r="B78" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="C78" s="10" t="s">
+      <c r="C78" s="36" t="s">
         <v>127</v>
       </c>
       <c r="D78" s="32"/>
@@ -4311,4 +4519,780 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId99"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5127F15-CE85-48F2-BB86-58B6FF85F56C}">
+  <dimension ref="A1:L62"/>
+  <sheetViews>
+    <sheetView topLeftCell="A5" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="50.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.90625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+      <c r="A1" s="39" t="s">
+        <v>255</v>
+      </c>
+      <c r="B1" s="38" t="s">
+        <v>276</v>
+      </c>
+      <c r="C1" s="38" t="s">
+        <v>254</v>
+      </c>
+      <c r="D1" s="38" t="s">
+        <v>275</v>
+      </c>
+      <c r="E1" s="39" t="s">
+        <v>273</v>
+      </c>
+      <c r="F1" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="39" t="s">
+        <v>274</v>
+      </c>
+      <c r="K1" s="38"/>
+      <c r="L1" s="39"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A2" s="41" t="s">
+        <v>143</v>
+      </c>
+      <c r="B2" s="40" t="s">
+        <v>256</v>
+      </c>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="K2" s="43"/>
+      <c r="L2" s="43"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3" s="41" t="s">
+        <v>144</v>
+      </c>
+      <c r="B3" s="40" t="s">
+        <v>256</v>
+      </c>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="K3" s="43"/>
+      <c r="L3" s="43"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A4" s="40" t="s">
+        <v>145</v>
+      </c>
+      <c r="B4" s="40" t="s">
+        <v>256</v>
+      </c>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="K4" s="43"/>
+      <c r="L4" s="43"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A5" s="43" t="s">
+        <v>233</v>
+      </c>
+      <c r="B5" s="43" t="s">
+        <v>183</v>
+      </c>
+      <c r="C5" s="43"/>
+      <c r="D5" s="43"/>
+      <c r="K5" s="43"/>
+      <c r="L5" s="43"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A6" s="43" t="s">
+        <v>103</v>
+      </c>
+      <c r="B6" s="43" t="s">
+        <v>183</v>
+      </c>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="K6" s="43"/>
+      <c r="L6" s="40"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A7" s="43" t="s">
+        <v>234</v>
+      </c>
+      <c r="B7" s="43" t="s">
+        <v>183</v>
+      </c>
+      <c r="C7" s="43"/>
+      <c r="D7" s="43"/>
+      <c r="K7" s="43"/>
+      <c r="L7" s="40"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A8" s="43" t="s">
+        <v>235</v>
+      </c>
+      <c r="B8" s="43" t="s">
+        <v>183</v>
+      </c>
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
+      <c r="K8" s="43"/>
+      <c r="L8" s="40"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A9" s="40" t="s">
+        <v>236</v>
+      </c>
+      <c r="B9" s="43" t="s">
+        <v>257</v>
+      </c>
+      <c r="C9" s="43"/>
+      <c r="D9" s="43"/>
+      <c r="K9" s="43"/>
+      <c r="L9" s="40"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A10" s="40" t="s">
+        <v>237</v>
+      </c>
+      <c r="B10" s="43" t="s">
+        <v>257</v>
+      </c>
+      <c r="C10" s="43"/>
+      <c r="D10" s="43"/>
+      <c r="K10" s="43"/>
+      <c r="L10" s="40"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A11" s="40" t="s">
+        <v>238</v>
+      </c>
+      <c r="B11" s="43" t="s">
+        <v>257</v>
+      </c>
+      <c r="C11" s="43"/>
+      <c r="D11" s="43"/>
+      <c r="K11" s="43"/>
+      <c r="L11" s="40"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A12" s="40" t="s">
+        <v>240</v>
+      </c>
+      <c r="B12" s="43" t="s">
+        <v>257</v>
+      </c>
+      <c r="C12" s="43"/>
+      <c r="D12" s="43"/>
+      <c r="K12" s="40"/>
+      <c r="L12" s="41"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A13" s="40" t="s">
+        <v>241</v>
+      </c>
+      <c r="B13" s="43" t="s">
+        <v>257</v>
+      </c>
+      <c r="C13" s="43"/>
+      <c r="D13" s="43"/>
+      <c r="K13" s="44"/>
+      <c r="L13" s="45"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A14" s="40" t="s">
+        <v>243</v>
+      </c>
+      <c r="B14" s="43" t="s">
+        <v>257</v>
+      </c>
+      <c r="C14" s="43"/>
+      <c r="D14" s="43"/>
+      <c r="K14" s="43"/>
+      <c r="L14" s="40"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A15" s="41" t="s">
+        <v>125</v>
+      </c>
+      <c r="B15" s="40" t="s">
+        <v>258</v>
+      </c>
+      <c r="C15" s="40"/>
+      <c r="D15" s="40"/>
+      <c r="K15" s="43"/>
+      <c r="L15" s="40"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A16" s="41" t="s">
+        <v>244</v>
+      </c>
+      <c r="B16" s="41" t="s">
+        <v>256</v>
+      </c>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
+      <c r="K16" s="43"/>
+      <c r="L16" s="40"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A17" s="41" t="s">
+        <v>150</v>
+      </c>
+      <c r="B17" s="40" t="s">
+        <v>260</v>
+      </c>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="K17" s="40"/>
+      <c r="L17" s="41"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A18" s="40" t="s">
+        <v>128</v>
+      </c>
+      <c r="B18" s="43" t="s">
+        <v>259</v>
+      </c>
+      <c r="C18" s="43"/>
+      <c r="D18" s="43"/>
+      <c r="K18" s="40"/>
+      <c r="L18" s="41"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A19" s="40" t="s">
+        <v>126</v>
+      </c>
+      <c r="B19" s="43" t="s">
+        <v>259</v>
+      </c>
+      <c r="C19" s="43"/>
+      <c r="D19" s="43"/>
+      <c r="K19" s="43"/>
+      <c r="L19" s="40"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A20" s="40" t="s">
+        <v>127</v>
+      </c>
+      <c r="B20" s="43" t="s">
+        <v>259</v>
+      </c>
+      <c r="C20" s="43"/>
+      <c r="D20" s="43"/>
+      <c r="K20" s="40"/>
+      <c r="L20" s="43"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A21" s="41" t="s">
+        <v>114</v>
+      </c>
+      <c r="B21" s="40" t="s">
+        <v>261</v>
+      </c>
+      <c r="C21" s="40"/>
+      <c r="D21" s="40"/>
+      <c r="K21" s="43"/>
+      <c r="L21" s="40"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A22" s="40" t="s">
+        <v>115</v>
+      </c>
+      <c r="B22" s="43" t="s">
+        <v>262</v>
+      </c>
+      <c r="C22" s="43"/>
+      <c r="D22" s="43"/>
+      <c r="K22" s="43"/>
+      <c r="L22" s="40"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A23" s="41" t="s">
+        <v>138</v>
+      </c>
+      <c r="B23" s="40" t="s">
+        <v>263</v>
+      </c>
+      <c r="C23" s="40"/>
+      <c r="D23" s="40"/>
+      <c r="K23" s="40"/>
+      <c r="L23" s="41"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A24" s="41" t="s">
+        <v>136</v>
+      </c>
+      <c r="B24" s="40" t="s">
+        <v>264</v>
+      </c>
+      <c r="C24" s="40"/>
+      <c r="D24" s="40"/>
+      <c r="K24" s="40"/>
+      <c r="L24" s="41"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A25" s="40" t="s">
+        <v>134</v>
+      </c>
+      <c r="B25" s="43" t="s">
+        <v>262</v>
+      </c>
+      <c r="C25" s="43"/>
+      <c r="D25" s="43"/>
+      <c r="K25" s="40"/>
+      <c r="L25" s="41"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A26" s="40" t="s">
+        <v>246</v>
+      </c>
+      <c r="B26" s="43" t="s">
+        <v>265</v>
+      </c>
+      <c r="C26" s="43"/>
+      <c r="D26" s="43"/>
+      <c r="K26" s="40"/>
+      <c r="L26" s="43"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A27" s="41" t="s">
+        <v>131</v>
+      </c>
+      <c r="B27" s="40" t="s">
+        <v>261</v>
+      </c>
+      <c r="C27" s="40"/>
+      <c r="D27" s="40"/>
+      <c r="K27" s="43"/>
+      <c r="L27" s="40"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A28" s="41" t="s">
+        <v>110</v>
+      </c>
+      <c r="B28" s="40" t="s">
+        <v>266</v>
+      </c>
+      <c r="C28" s="40"/>
+      <c r="D28" s="40"/>
+      <c r="K28" s="43"/>
+      <c r="L28" s="43"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A29" s="43" t="s">
+        <v>101</v>
+      </c>
+      <c r="B29" s="43" t="s">
+        <v>183</v>
+      </c>
+      <c r="C29" s="43"/>
+      <c r="D29" s="43"/>
+      <c r="K29" s="40"/>
+      <c r="L29" s="41"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A30" s="41" t="s">
+        <v>100</v>
+      </c>
+      <c r="B30" s="40" t="s">
+        <v>183</v>
+      </c>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="K30" s="43"/>
+      <c r="L30" s="40"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A31" s="43" t="s">
+        <v>102</v>
+      </c>
+      <c r="B31" s="43" t="s">
+        <v>183</v>
+      </c>
+      <c r="C31" s="43"/>
+      <c r="D31" s="43"/>
+      <c r="K31" s="43"/>
+      <c r="L31" s="40"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A32" s="40" t="s">
+        <v>111</v>
+      </c>
+      <c r="B32" s="43" t="s">
+        <v>267</v>
+      </c>
+      <c r="C32" s="43"/>
+      <c r="D32" s="43"/>
+      <c r="K32" s="43"/>
+      <c r="L32" s="40"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A33" s="40" t="s">
+        <v>116</v>
+      </c>
+      <c r="B33" s="43" t="s">
+        <v>267</v>
+      </c>
+      <c r="C33" s="43"/>
+      <c r="D33" s="43"/>
+      <c r="K33" s="43"/>
+      <c r="L33" s="40"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A34" s="40" t="s">
+        <v>117</v>
+      </c>
+      <c r="B34" s="43" t="s">
+        <v>267</v>
+      </c>
+      <c r="C34" s="43"/>
+      <c r="D34" s="43"/>
+      <c r="K34" s="40"/>
+      <c r="L34" s="41"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A35" s="41" t="s">
+        <v>120</v>
+      </c>
+      <c r="B35" s="40" t="s">
+        <v>183</v>
+      </c>
+      <c r="C35" s="40"/>
+      <c r="D35" s="40"/>
+      <c r="K35" s="40"/>
+      <c r="L35" s="41"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A36" s="41" t="s">
+        <v>121</v>
+      </c>
+      <c r="B36" s="40" t="s">
+        <v>262</v>
+      </c>
+      <c r="C36" s="40"/>
+      <c r="D36" s="40"/>
+      <c r="K36" s="43"/>
+      <c r="L36" s="43"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A37" s="41" t="s">
+        <v>122</v>
+      </c>
+      <c r="B37" s="40" t="s">
+        <v>262</v>
+      </c>
+      <c r="C37" s="40"/>
+      <c r="D37" s="40"/>
+      <c r="K37" s="43"/>
+      <c r="L37" s="43"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A38" s="41" t="s">
+        <v>124</v>
+      </c>
+      <c r="B38" s="40" t="s">
+        <v>262</v>
+      </c>
+      <c r="C38" s="40"/>
+      <c r="D38" s="40"/>
+      <c r="K38" s="40"/>
+      <c r="L38" s="43"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A39" s="41" t="s">
+        <v>118</v>
+      </c>
+      <c r="B39" s="40" t="s">
+        <v>268</v>
+      </c>
+      <c r="C39" s="40"/>
+      <c r="D39" s="40"/>
+      <c r="K39" s="40"/>
+      <c r="L39" s="41"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A40" s="41" t="s">
+        <v>109</v>
+      </c>
+      <c r="B40" s="40" t="s">
+        <v>269</v>
+      </c>
+      <c r="C40" s="40"/>
+      <c r="D40" s="40"/>
+      <c r="K40" s="40"/>
+      <c r="L40" s="41"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A41" s="40" t="s">
+        <v>119</v>
+      </c>
+      <c r="B41" s="43" t="s">
+        <v>267</v>
+      </c>
+      <c r="C41" s="43"/>
+      <c r="D41" s="43"/>
+      <c r="K41" s="40"/>
+      <c r="L41" s="41"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A42" s="43" t="s">
+        <v>104</v>
+      </c>
+      <c r="B42" s="43" t="s">
+        <v>183</v>
+      </c>
+      <c r="C42" s="43"/>
+      <c r="D42" s="43"/>
+      <c r="K42" s="40"/>
+      <c r="L42" s="41"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A43" s="43" t="s">
+        <v>106</v>
+      </c>
+      <c r="B43" s="43" t="s">
+        <v>183</v>
+      </c>
+      <c r="C43" s="43"/>
+      <c r="D43" s="43"/>
+      <c r="K43" s="40"/>
+      <c r="L43" s="41"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A44" s="43" t="s">
+        <v>107</v>
+      </c>
+      <c r="B44" s="43" t="s">
+        <v>183</v>
+      </c>
+      <c r="C44" s="43"/>
+      <c r="D44" s="43"/>
+      <c r="K44" s="42"/>
+      <c r="L44" s="42"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A45" s="43" t="s">
+        <v>105</v>
+      </c>
+      <c r="B45" s="43" t="s">
+        <v>183</v>
+      </c>
+      <c r="C45" s="43"/>
+      <c r="D45" s="43"/>
+      <c r="K45" s="41"/>
+      <c r="L45" s="41"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A46" s="43" t="s">
+        <v>108</v>
+      </c>
+      <c r="B46" s="40" t="s">
+        <v>269</v>
+      </c>
+      <c r="C46" s="40"/>
+      <c r="D46" s="40"/>
+      <c r="K46" s="43"/>
+      <c r="L46" s="43"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A47" s="43" t="s">
+        <v>245</v>
+      </c>
+      <c r="B47" s="40" t="s">
+        <v>261</v>
+      </c>
+      <c r="C47" s="40"/>
+      <c r="D47" s="40"/>
+      <c r="K47" s="43"/>
+      <c r="L47" s="43"/>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A48" s="43" t="s">
+        <v>248</v>
+      </c>
+      <c r="B48" s="43" t="s">
+        <v>270</v>
+      </c>
+      <c r="C48" s="43"/>
+      <c r="D48" s="43"/>
+      <c r="K48" s="43"/>
+      <c r="L48" s="43"/>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A49" s="43" t="s">
+        <v>249</v>
+      </c>
+      <c r="B49" s="43" t="s">
+        <v>270</v>
+      </c>
+      <c r="C49" s="43"/>
+      <c r="D49" s="43"/>
+      <c r="K49" s="43"/>
+      <c r="L49" s="43"/>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A50" s="43" t="s">
+        <v>250</v>
+      </c>
+      <c r="B50" s="43" t="s">
+        <v>270</v>
+      </c>
+      <c r="C50" s="43"/>
+      <c r="D50" s="43"/>
+      <c r="K50" s="43"/>
+      <c r="L50" s="43"/>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A51" s="43" t="s">
+        <v>242</v>
+      </c>
+      <c r="B51" s="43" t="s">
+        <v>271</v>
+      </c>
+      <c r="C51" s="43"/>
+      <c r="D51" s="43"/>
+      <c r="K51" s="43"/>
+      <c r="L51" s="43"/>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A52" s="43" t="s">
+        <v>239</v>
+      </c>
+      <c r="B52" s="43" t="s">
+        <v>271</v>
+      </c>
+      <c r="C52" s="43"/>
+      <c r="D52" s="43"/>
+      <c r="K52" s="43"/>
+      <c r="L52" s="43"/>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A53" s="43" t="s">
+        <v>123</v>
+      </c>
+      <c r="B53" s="43" t="s">
+        <v>272</v>
+      </c>
+      <c r="C53" s="43"/>
+      <c r="D53" s="43"/>
+      <c r="K53" s="43"/>
+      <c r="L53" s="43"/>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A54" s="43" t="s">
+        <v>247</v>
+      </c>
+      <c r="B54" s="40" t="s">
+        <v>262</v>
+      </c>
+      <c r="C54" s="40"/>
+      <c r="D54" s="40"/>
+      <c r="K54" s="40"/>
+      <c r="L54" s="41"/>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>251</v>
+      </c>
+      <c r="B55" s="43" t="s">
+        <v>181</v>
+      </c>
+      <c r="C55" s="43"/>
+      <c r="D55" s="43"/>
+      <c r="K55" s="43"/>
+      <c r="L55" s="43"/>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>252</v>
+      </c>
+      <c r="B56" s="43" t="s">
+        <v>181</v>
+      </c>
+      <c r="C56" s="43"/>
+      <c r="D56" s="43"/>
+      <c r="K56" s="40"/>
+      <c r="L56" s="41"/>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>253</v>
+      </c>
+      <c r="B57" s="43" t="s">
+        <v>181</v>
+      </c>
+      <c r="C57" s="43"/>
+      <c r="D57" s="43"/>
+      <c r="K57" s="43"/>
+      <c r="L57" s="43"/>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>172</v>
+      </c>
+      <c r="B58" s="43" t="s">
+        <v>181</v>
+      </c>
+      <c r="C58" s="43"/>
+      <c r="D58" s="43"/>
+      <c r="K58" s="43"/>
+      <c r="L58" s="43"/>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>167</v>
+      </c>
+      <c r="B59" s="43" t="s">
+        <v>181</v>
+      </c>
+      <c r="C59" s="43"/>
+      <c r="D59" s="43"/>
+      <c r="K59" s="43"/>
+      <c r="L59" s="43"/>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>168</v>
+      </c>
+      <c r="B60" s="43" t="s">
+        <v>181</v>
+      </c>
+      <c r="C60" s="43"/>
+      <c r="D60" s="43"/>
+      <c r="K60" s="43"/>
+      <c r="L60" s="43"/>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>169</v>
+      </c>
+      <c r="B61" s="43" t="s">
+        <v>181</v>
+      </c>
+      <c r="C61" s="43"/>
+      <c r="D61" s="43"/>
+      <c r="K61" s="43"/>
+      <c r="L61" s="43"/>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>170</v>
+      </c>
+      <c r="B62" s="43" t="s">
+        <v>181</v>
+      </c>
+      <c r="C62" s="43"/>
+      <c r="D62" s="43"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>